<commit_message>
Made tweaks to GUI_new.py
</commit_message>
<xml_diff>
--- a/RITM_INC_CHG-Details.xlsx
+++ b/RITM_INC_CHG-Details.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbjt_baki/Desktop/Data_Engineering/Metathon/METATHON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7555FE0-3763-8945-8507-883F098CD6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2D966-6FEE-1643-9877-220C4F1E6C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" xr2:uid="{54A95667-31C6-4D40-9237-4FD7C7CD00C8}"/>
+    <workbookView xWindow="2320" yWindow="500" windowWidth="18160" windowHeight="12300" xr2:uid="{54A95667-31C6-4D40-9237-4FD7C7CD00C8}"/>
   </bookViews>
   <sheets>
-    <sheet name="RITM Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="INC Sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="RITM_Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="INC_Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -870,7 +870,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1981,7 +1981,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>